<commit_message>
Added methods for testing targets
Added methods in BoardAdjTargetTest to test for calculated targets
</commit_message>
<xml_diff>
--- a/layout/ClueLayoutTests.xlsx
+++ b/layout/ClueLayoutTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\millw\CSCI 306 Workspace\ClueGame\layout\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590191E0-8F76-4B61-A9FA-D3F40B88F214}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6BD3CE0-2F42-414F-9B74-66DE9A0251C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="49">
   <si>
     <t>X</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Red - Test Occupied</t>
+  </si>
+  <si>
+    <t>Notes: Cell E* also used for light orange</t>
   </si>
 </sst>
 </file>
@@ -223,7 +226,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -366,6 +369,36 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFAE5D"/>
         <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81E1FF"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81E1FF"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF81E1FF"/>
+        <bgColor rgb="FFB6D7A8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFFE599"/>
       </patternFill>
     </fill>
   </fills>
@@ -381,7 +414,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -440,8 +473,17 @@
     <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +492,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF81E1FF"/>
       <color rgb="FFFFAE5D"/>
       <color rgb="FFFFC081"/>
       <color rgb="FFE26100"/>
-      <color rgb="FF81E1FF"/>
       <color rgb="FFA3C2FF"/>
     </mruColors>
   </colors>
@@ -672,7 +714,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -927,7 +969,7 @@
       <c r="V3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="57" t="s">
+      <c r="W3" s="56" t="s">
         <v>5</v>
       </c>
       <c r="X3" s="48" t="s">
@@ -1122,7 +1164,7 @@
       <c r="G6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="60" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="12" t="s">
@@ -1307,7 +1349,7 @@
       <c r="P8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="Q8" s="61" t="s">
         <v>17</v>
       </c>
       <c r="R8" s="6" t="s">
@@ -1369,7 +1411,7 @@
       <c r="J9" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="K9" s="44" t="s">
         <v>1</v>
       </c>
       <c r="L9" s="13" t="s">
@@ -1571,7 +1613,7 @@
       <c r="X11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y11" s="5" t="s">
+      <c r="Y11" s="62" t="s">
         <v>1</v>
       </c>
       <c r="AA11" s="29"/>
@@ -1646,11 +1688,14 @@
       <c r="W12" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="X12" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="5" t="s">
-        <v>1</v>
+      <c r="X12" s="62" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="63" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="59" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
@@ -1726,7 +1771,7 @@
       <c r="X13" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="Y13" s="5" t="s">
+      <c r="Y13" s="64" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1788,7 +1833,7 @@
       <c r="S14" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="T14" s="8" t="s">
+      <c r="T14" s="57" t="s">
         <v>10</v>
       </c>
       <c r="U14" s="14" t="s">
@@ -2004,7 +2049,7 @@
       <c r="N17" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="O17" s="31" t="s">
+      <c r="O17" s="65" t="s">
         <v>24</v>
       </c>
       <c r="P17" s="7" t="s">
@@ -2069,10 +2114,10 @@
       <c r="J18" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="K18" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="8" t="s">
+      <c r="L18" s="66" t="s">
         <v>24</v>
       </c>
       <c r="M18" s="7" t="s">
@@ -2241,7 +2286,7 @@
       <c r="P20" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q20" s="9" t="s">
+      <c r="Q20" s="61" t="s">
         <v>28</v>
       </c>
       <c r="R20" s="6" t="s">
@@ -2473,13 +2518,13 @@
       <c r="P23" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="Q23" s="65" t="s">
         <v>10</v>
       </c>
       <c r="R23" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="S23" s="5" t="s">
+      <c r="S23" s="58" t="s">
         <v>1</v>
       </c>
       <c r="T23" s="44" t="s">
@@ -2488,7 +2533,7 @@
       <c r="U23" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="V23" s="19" t="s">
+      <c r="V23" s="6" t="s">
         <v>29</v>
       </c>
       <c r="W23" s="52" t="s">
@@ -2551,7 +2596,7 @@
       <c r="P24" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q24" s="65" t="s">
         <v>10</v>
       </c>
       <c r="R24" s="5" t="s">

</xml_diff>